<commit_message>
mise à jour des activités
</commit_message>
<xml_diff>
--- a/conversion.xlsx
+++ b/conversion.xlsx
@@ -1,39 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benoit Beroule\Dropbox\Oiseau-Rare\Projets\Meetup\ConversionDeDevises\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\RPA\ConversionDeDevises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC67608-0B9D-46BA-A3A5-E55F9D00F523}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B6EC57-6470-4E84-9773-5D02311B33A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EBAFD9D6-D9B7-453B-8864-565A082746BA}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{EBAFD9D6-D9B7-453B-8864-565A082746BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="12">
   <si>
     <t>valeurDeBase</t>
   </si>
@@ -66,6 +58,9 @@
   </si>
   <si>
     <t>resultat</t>
+  </si>
+  <si>
+    <t>0,55008</t>
   </si>
 </sst>
 </file>
@@ -480,7 +475,9 @@
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2">

</xml_diff>